<commit_message>
More study stuff n=1
</commit_message>
<xml_diff>
--- a/n of 1/My n of 1/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-2.xlsx
+++ b/n of 1/My n of 1/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="240" windowWidth="25875" windowHeight="10680" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="25875" windowHeight="10680" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="VO2max" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>METS</t>
   </si>
@@ -119,11 +119,22 @@
   <si>
     <t>CHO Ox kcal/min</t>
   </si>
+  <si>
+    <t>CHO Ox 
+kcal/min</t>
+  </si>
+  <si>
+    <t>Fat Ox 
+kcal/min</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -563,6 +574,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -609,7 +635,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -619,6 +645,14 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1034,11 +1068,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49090560"/>
-        <c:axId val="49092096"/>
+        <c:axId val="125174144"/>
+        <c:axId val="125175680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49090560"/>
+        <c:axId val="125174144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1052,12 +1086,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49092096"/>
+        <c:crossAx val="125175680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49092096"/>
+        <c:axId val="125175680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1103,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49090560"/>
+        <c:crossAx val="125174144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1486,11 +1520,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49138304"/>
-        <c:axId val="49144192"/>
+        <c:axId val="125217792"/>
+        <c:axId val="125223680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49138304"/>
+        <c:axId val="125217792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -1504,12 +1538,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49144192"/>
+        <c:crossAx val="125223680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49144192"/>
+        <c:axId val="125223680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1522,7 +1556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49138304"/>
+        <c:crossAx val="125217792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1959,11 +1993,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49346816"/>
-        <c:axId val="49414144"/>
+        <c:axId val="125119104"/>
+        <c:axId val="125129088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49346816"/>
+        <c:axId val="125119104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1977,12 +2011,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49414144"/>
+        <c:crossAx val="125129088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49414144"/>
+        <c:axId val="125129088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +2028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49346816"/>
+        <c:crossAx val="125119104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2770,11 +2804,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49455488"/>
-        <c:axId val="49457024"/>
+        <c:axId val="125248256"/>
+        <c:axId val="125249792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49455488"/>
+        <c:axId val="125248256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -2787,12 +2821,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49457024"/>
+        <c:crossAx val="125249792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49457024"/>
+        <c:axId val="125249792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2806,7 +2840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49455488"/>
+        <c:crossAx val="125248256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2817,10 +2851,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14138324966380847"/>
-          <c:y val="0.12190132545662116"/>
-          <c:w val="0.17986880964426397"/>
-          <c:h val="0.31392076677080683"/>
+          <c:x val="6.8466617454068235E-2"/>
+          <c:y val="5.6921565282040718E-2"/>
+          <c:w val="0.29271598862642167"/>
+          <c:h val="0.21145275621464074"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2871,7 +2905,8 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fat Ox kcal/min</c:v>
+                  <c:v>Fat Ox 
+kcal/min</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2944,264 +2979,240 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'CHR-FAT_HR'!$A$2:$A$42</c:f>
+              <c:f>'CHR-FAT_HR'!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>78</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>76</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>76</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>84</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>88</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>94</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>96</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>99</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>102</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>103</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>106</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>114</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>106</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>109</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>117</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>124</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>126</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>129</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>135</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>138</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>148</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>139</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>143</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>149</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>155</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>158</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>161</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>165</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'CHR-FAT_HR'!$B$2:$B$42</c:f>
+              <c:f>'CHR-FAT_HR'!$B$2:$B$39</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>1.9452959999999999</c:v>
+                  <c:v>1.4088959999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2091199999999995</c:v>
+                  <c:v>1.6511039999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3446719999999994</c:v>
+                  <c:v>1.7075999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4088959999999997</c:v>
+                  <c:v>2.9329439999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6511039999999997</c:v>
+                  <c:v>3.5287199999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7075999999999996</c:v>
+                  <c:v>2.809056</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9329439999999996</c:v>
+                  <c:v>3.4027199999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5287199999999999</c:v>
+                  <c:v>4.8094079999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.809056</c:v>
+                  <c:v>4.878671999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4027199999999991</c:v>
+                  <c:v>5.8661279999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.8094079999999995</c:v>
+                  <c:v>5.9334719999999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.878671999999999</c:v>
+                  <c:v>7.9756799999999988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.8661279999999998</c:v>
+                  <c:v>9.7514400000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9334719999999992</c:v>
+                  <c:v>9.1929599999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.9756799999999988</c:v>
+                  <c:v>11.114880000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.7514400000000006</c:v>
+                  <c:v>10.528128000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1929599999999994</c:v>
+                  <c:v>8.8490879999999983</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.114880000000003</c:v>
+                  <c:v>9.9859199999999984</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.528128000000002</c:v>
+                  <c:v>11.872559999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.8490879999999983</c:v>
+                  <c:v>10.959839999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9859199999999984</c:v>
+                  <c:v>10.771055999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.872559999999998</c:v>
+                  <c:v>9.178799999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.959839999999998</c:v>
+                  <c:v>9.6455999999999964</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.771055999999998</c:v>
+                  <c:v>10.481375999999996</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.178799999999999</c:v>
+                  <c:v>7.8321599999999991</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.6455999999999964</c:v>
+                  <c:v>8.0180159999999994</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10.481375999999996</c:v>
+                  <c:v>6.9573119999999991</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.8321599999999991</c:v>
+                  <c:v>8.2974719999999973</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.0180159999999994</c:v>
+                  <c:v>5.2545599999999952</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.9573119999999991</c:v>
+                  <c:v>3.7339679999999928</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.2974719999999973</c:v>
+                  <c:v>2.3767679999999993</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.2545599999999952</c:v>
+                  <c:v>0.58747199999999777</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.7339679999999928</c:v>
+                  <c:v>-2.4595200000000075</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3767679999999993</c:v>
+                  <c:v>-2.5288320000000075</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.58747199999999777</c:v>
+                  <c:v>-5.0465280000000075</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-2.4595200000000075</c:v>
+                  <c:v>-4.6958400000000076</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-2.5288320000000075</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>-5.0465280000000075</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>-4.6958400000000076</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>-4.7266560000000073</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>-3.2699040000000039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3217,7 +3228,8 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CHO Ox kcal/min</c:v>
+                  <c:v>CHO Ox 
+kcal/min</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3235,8 +3247,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.3413027916964926E-2"/>
-                  <c:y val="-7.5662491742579394E-3"/>
+                  <c:x val="5.0182068959443972E-2"/>
+                  <c:y val="-6.0539436206068685E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -3290,264 +3302,240 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'CHR-FAT_HR'!$A$2:$A$42</c:f>
+              <c:f>'CHR-FAT_HR'!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>78</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>76</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>76</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>84</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>92</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>84</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>88</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>90</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>94</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>96</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>99</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>102</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>103</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>106</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>114</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>106</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>109</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>117</c:v>
+                  <c:v>129</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>124</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>126</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>129</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>135</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>138</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>148</c:v>
+                  <c:v>149</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>139</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>143</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>149</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>155</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>158</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>161</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>165</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>167</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>169</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>170</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>161</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'CHR-FAT_HR'!$C$2:$C$42</c:f>
+              <c:f>'CHR-FAT_HR'!$C$2:$C$39</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0.21614400000000022</c:v>
+                  <c:v>0.35222400000000031</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43968000000000046</c:v>
+                  <c:v>0.25401600000000041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57628800000000047</c:v>
+                  <c:v>0.34152000000000032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35222400000000031</c:v>
+                  <c:v>0.10113599999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25401600000000041</c:v>
+                  <c:v>0.12167999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34152000000000032</c:v>
+                  <c:v>9.6863999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10113599999999996</c:v>
+                  <c:v>-0.40031999999999923</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.12167999999999997</c:v>
+                  <c:v>-0.90988799999999925</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.6863999999999978E-2</c:v>
+                  <c:v>-0.92299199999999926</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.40031999999999923</c:v>
+                  <c:v>-1.1098079999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.90988799999999925</c:v>
+                  <c:v>-1.2491519999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.92299199999999926</c:v>
+                  <c:v>-1.9939199999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.1098079999999992</c:v>
+                  <c:v>-2.6162400000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.2491519999999996</c:v>
+                  <c:v>-2.2982399999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.9939199999999995</c:v>
+                  <c:v>-2.7787199999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.6162400000000003</c:v>
+                  <c:v>-2.2164479999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.2982399999999998</c:v>
+                  <c:v>-1.4748479999999982</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.7787199999999999</c:v>
+                  <c:v>-1.4265599999999987</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.2164479999999998</c:v>
+                  <c:v>-1.6960799999999985</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.4748479999999982</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.4265599999999987</c:v>
+                  <c:v>1.196784000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-1.6960799999999985</c:v>
+                  <c:v>1.8357600000000023</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1.9291200000000019</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.196784000000001</c:v>
+                  <c:v>3.1899840000000039</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.8357600000000023</c:v>
+                  <c:v>5.2214400000000003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.9291200000000019</c:v>
+                  <c:v>6.131424</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.1899840000000039</c:v>
+                  <c:v>6.0876480000000024</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.2214400000000003</c:v>
+                  <c:v>7.2602880000000019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.131424</c:v>
+                  <c:v>10.509120000000005</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.0876480000000024</c:v>
+                  <c:v>12.268752000000003</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.2602880000000019</c:v>
+                  <c:v>15.448992000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10.509120000000005</c:v>
+                  <c:v>17.036688000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>12.268752000000003</c:v>
+                  <c:v>20.905920000000009</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15.448992000000002</c:v>
+                  <c:v>21.495072000000008</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>17.036688000000002</c:v>
+                  <c:v>23.971008000000005</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20.905920000000009</c:v>
+                  <c:v>20.348640000000007</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>21.495072000000008</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>23.971008000000005</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>20.348640000000007</c:v>
-                </c:pt>
-                <c:pt idx="39">
                   <c:v>22.451616000000005</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>12.187824000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3562,14 +3550,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50342912"/>
-        <c:axId val="50356992"/>
+        <c:axId val="125401344"/>
+        <c:axId val="125411328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50342912"/>
+        <c:axId val="125401344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="60"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3578,12 +3566,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50356992"/>
+        <c:crossAx val="125411328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50356992"/>
+        <c:axId val="125411328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3591,11 +3579,11 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:minorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50342912"/>
+        <c:crossAx val="125401344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3606,10 +3594,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.29289827407937646"/>
-          <c:y val="0.79295851475676082"/>
-          <c:w val="0.19900564720831754"/>
-          <c:h val="0.14027953837548154"/>
+          <c:x val="6.5724802877878394E-2"/>
+          <c:y val="0.18858007281677866"/>
+          <c:w val="0.46462383055918499"/>
+          <c:h val="0.13781266850340232"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3697,114 +3685,111 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.12280701754385964</c:v>
+                  <c:v>9.0643274853801165E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0643274853801165E-2</c:v>
+                  <c:v>0.10818713450292397</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10818713450292397</c:v>
+                  <c:v>9.6491228070175419E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6491228070175419E-2</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10526315789473684</c:v>
+                  <c:v>0.11695906432748537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11695906432748537</c:v>
+                  <c:v>0.17251461988304093</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.20760233918128651</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.17251461988304093</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.20760233918128651</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.16666666666666666</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17251461988304093</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22807017543859648</c:v>
+                  <c:v>0.27777777777777773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27777777777777773</c:v>
+                  <c:v>0.27192982456140352</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27192982456140352</c:v>
+                  <c:v>0.34795321637426901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.34795321637426901</c:v>
+                  <c:v>0.41812865497076024</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.41812865497076024</c:v>
+                  <c:v>0.40350877192982454</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.40350877192982454</c:v>
+                  <c:v>0.48538011695906436</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.48538011695906436</c:v>
+                  <c:v>0.48245614035087714</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.48245614035087714</c:v>
+                  <c:v>0.42690058479532161</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.42690058479532161</c:v>
+                  <c:v>0.49122807017543857</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.49122807017543857</c:v>
+                  <c:v>0.58771929824561397</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.58771929824561397</c:v>
+                  <c:v>0.62573099415204669</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.62573099415204669</c:v>
+                  <c:v>0.67836257309941517</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.67836257309941517</c:v>
+                  <c:v>0.62280701754385959</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.62280701754385959</c:v>
+                  <c:v>0.64912280701754377</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.64912280701754377</c:v>
+                  <c:v>0.76608187134502914</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.76608187134502914</c:v>
+                  <c:v>0.72514619883040932</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.72514619883040932</c:v>
+                  <c:v>0.78070175438596479</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.78070175438596479</c:v>
+                  <c:v>0.7192982456140351</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.7192982456140351</c:v>
+                  <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.85964912280701744</c:v>
+                  <c:v>0.86257309941520466</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.86257309941520466</c:v>
+                  <c:v>0.95614035087719296</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.95614035087719296</c:v>
+                  <c:v>0.9385964912280701</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.9385964912280701</c:v>
+                  <c:v>0.97076023391812871</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.97076023391812871</c:v>
-                </c:pt>
-                <c:pt idx="36">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3817,114 +3802,111 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>1.9452959999999999</c:v>
+                  <c:v>1.2091199999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2091199999999995</c:v>
+                  <c:v>1.3446719999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3446719999999994</c:v>
+                  <c:v>1.4088959999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4088959999999997</c:v>
+                  <c:v>1.6511039999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6511039999999997</c:v>
+                  <c:v>1.7075999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7075999999999996</c:v>
+                  <c:v>2.9329439999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9329439999999996</c:v>
+                  <c:v>3.5287199999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.5287199999999999</c:v>
+                  <c:v>2.809056</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.809056</c:v>
+                  <c:v>3.4027199999999991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4027199999999991</c:v>
+                  <c:v>4.8094079999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.8094079999999995</c:v>
+                  <c:v>4.878671999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.878671999999999</c:v>
+                  <c:v>5.8661279999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.8661279999999998</c:v>
+                  <c:v>5.9334719999999992</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9334719999999992</c:v>
+                  <c:v>7.9756799999999988</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.9756799999999988</c:v>
+                  <c:v>9.7514400000000006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.7514400000000006</c:v>
+                  <c:v>9.1929599999999994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1929599999999994</c:v>
+                  <c:v>11.114880000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.114880000000003</c:v>
+                  <c:v>10.528128000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.528128000000002</c:v>
+                  <c:v>8.8490879999999983</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.8490879999999983</c:v>
+                  <c:v>9.9859199999999984</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9859199999999984</c:v>
+                  <c:v>11.872559999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>11.872559999999998</c:v>
+                  <c:v>10.959839999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.959839999999998</c:v>
+                  <c:v>10.771055999999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.771055999999998</c:v>
+                  <c:v>9.178799999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.178799999999999</c:v>
+                  <c:v>9.6455999999999964</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.6455999999999964</c:v>
+                  <c:v>10.481375999999996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10.481375999999996</c:v>
+                  <c:v>7.8321599999999991</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.8321599999999991</c:v>
+                  <c:v>8.0180159999999994</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.0180159999999994</c:v>
+                  <c:v>6.9573119999999991</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.9573119999999991</c:v>
+                  <c:v>8.2974719999999973</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.2974719999999973</c:v>
+                  <c:v>5.2545599999999952</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.2545599999999952</c:v>
+                  <c:v>3.7339679999999928</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.7339679999999928</c:v>
+                  <c:v>2.3767679999999993</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.3767679999999993</c:v>
+                  <c:v>0.58747199999999777</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.58747199999999777</c:v>
+                  <c:v>-2.4595200000000075</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-2.4595200000000075</c:v>
-                </c:pt>
-                <c:pt idx="36">
                   <c:v>-2.5288320000000075</c:v>
                 </c:pt>
               </c:numCache>
@@ -3978,114 +3960,111 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.12280701754385964</c:v>
+                  <c:v>9.0643274853801165E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0643274853801165E-2</c:v>
+                  <c:v>0.10818713450292397</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10818713450292397</c:v>
+                  <c:v>9.6491228070175419E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6491228070175419E-2</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10526315789473684</c:v>
+                  <c:v>0.11695906432748537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11695906432748537</c:v>
+                  <c:v>0.17251461988304093</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.20760233918128651</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.17251461988304093</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.20760233918128651</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.16666666666666666</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17251461988304093</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.22807017543859648</c:v>
+                  <c:v>0.27777777777777773</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27777777777777773</c:v>
+                  <c:v>0.27192982456140352</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27192982456140352</c:v>
+                  <c:v>0.34795321637426901</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.34795321637426901</c:v>
+                  <c:v>0.41812865497076024</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.41812865497076024</c:v>
+                  <c:v>0.40350877192982454</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.40350877192982454</c:v>
+                  <c:v>0.48538011695906436</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.48538011695906436</c:v>
+                  <c:v>0.48245614035087714</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.48245614035087714</c:v>
+                  <c:v>0.42690058479532161</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.42690058479532161</c:v>
+                  <c:v>0.49122807017543857</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.49122807017543857</c:v>
+                  <c:v>0.58771929824561397</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.58771929824561397</c:v>
+                  <c:v>0.62573099415204669</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.62573099415204669</c:v>
+                  <c:v>0.67836257309941517</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.67836257309941517</c:v>
+                  <c:v>0.62280701754385959</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.62280701754385959</c:v>
+                  <c:v>0.64912280701754377</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.64912280701754377</c:v>
+                  <c:v>0.76608187134502914</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.76608187134502914</c:v>
+                  <c:v>0.72514619883040932</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.72514619883040932</c:v>
+                  <c:v>0.78070175438596479</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.78070175438596479</c:v>
+                  <c:v>0.7192982456140351</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.7192982456140351</c:v>
+                  <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.85964912280701744</c:v>
+                  <c:v>0.86257309941520466</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.86257309941520466</c:v>
+                  <c:v>0.95614035087719296</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.95614035087719296</c:v>
+                  <c:v>0.9385964912280701</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.9385964912280701</c:v>
+                  <c:v>0.97076023391812871</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.97076023391812871</c:v>
-                </c:pt>
-                <c:pt idx="36">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -4098,114 +4077,111 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.21614400000000022</c:v>
+                  <c:v>0.43968000000000046</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43968000000000046</c:v>
+                  <c:v>0.57628800000000047</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57628800000000047</c:v>
+                  <c:v>0.35222400000000031</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35222400000000031</c:v>
+                  <c:v>0.25401600000000041</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25401600000000041</c:v>
+                  <c:v>0.34152000000000032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.34152000000000032</c:v>
+                  <c:v>0.10113599999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10113599999999996</c:v>
+                  <c:v>0.12167999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.12167999999999997</c:v>
+                  <c:v>9.6863999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.6863999999999978E-2</c:v>
+                  <c:v>-0.40031999999999923</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.40031999999999923</c:v>
+                  <c:v>-0.90988799999999925</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.90988799999999925</c:v>
+                  <c:v>-0.92299199999999926</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.92299199999999926</c:v>
+                  <c:v>-1.1098079999999992</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.1098079999999992</c:v>
+                  <c:v>-1.2491519999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.2491519999999996</c:v>
+                  <c:v>-1.9939199999999995</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-1.9939199999999995</c:v>
+                  <c:v>-2.6162400000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.6162400000000003</c:v>
+                  <c:v>-2.2982399999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.2982399999999998</c:v>
+                  <c:v>-2.7787199999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.7787199999999999</c:v>
+                  <c:v>-2.2164479999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.2164479999999998</c:v>
+                  <c:v>-1.4748479999999982</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.4748479999999982</c:v>
+                  <c:v>-1.4265599999999987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.4265599999999987</c:v>
+                  <c:v>-1.6960799999999985</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-1.6960799999999985</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>1.196784000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.196784000000001</c:v>
+                  <c:v>1.8357600000000023</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.8357600000000023</c:v>
+                  <c:v>1.9291200000000019</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.9291200000000019</c:v>
+                  <c:v>3.1899840000000039</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.1899840000000039</c:v>
+                  <c:v>5.2214400000000003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.2214400000000003</c:v>
+                  <c:v>6.131424</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.131424</c:v>
+                  <c:v>6.0876480000000024</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.0876480000000024</c:v>
+                  <c:v>7.2602880000000019</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.2602880000000019</c:v>
+                  <c:v>10.509120000000005</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10.509120000000005</c:v>
+                  <c:v>12.268752000000003</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>12.268752000000003</c:v>
+                  <c:v>15.448992000000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15.448992000000002</c:v>
+                  <c:v>17.036688000000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>17.036688000000002</c:v>
+                  <c:v>20.905920000000009</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20.905920000000009</c:v>
-                </c:pt>
-                <c:pt idx="36">
                   <c:v>21.495072000000008</c:v>
                 </c:pt>
               </c:numCache>
@@ -4221,11 +4197,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="50070656"/>
-        <c:axId val="50072192"/>
+        <c:axId val="126754816"/>
+        <c:axId val="126756352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50070656"/>
+        <c:axId val="126754816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4237,12 +4213,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50072192"/>
+        <c:crossAx val="126756352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50072192"/>
+        <c:axId val="126756352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4254,7 +4230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50070656"/>
+        <c:crossAx val="126754816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4457,6 +4433,186 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="462884" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="381000"/>
+          <a:ext cx="462884" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>kcal/</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>min</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="923925" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7496174" y="3752850"/>
+          <a:ext cx="923925" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Heart Rate</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>(bpm)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="923925" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7400924" y="1724025"/>
+          <a:ext cx="923925" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Heart Rate</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>(bpm)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4785,7 +4941,7 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8301,7 +8457,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:O1048576"/>
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9125,7 +9281,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9729,602 +9885,546 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="str">
         <f>VO2max!M4</f>
         <v>HR
 bpm</v>
       </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>VO2max!M5</f>
-        <v>78</v>
-      </c>
-      <c r="B2">
-        <f>VO2max!T5*9</f>
-        <v>1.9452959999999999</v>
-      </c>
-      <c r="C2">
-        <f>VO2max!U5*4</f>
-        <v>0.21614400000000022</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>VO2max!M6</f>
-        <v>76</v>
-      </c>
-      <c r="B3">
-        <f>VO2max!T6*9</f>
-        <v>1.2091199999999995</v>
-      </c>
-      <c r="C3">
-        <f>VO2max!U6*4</f>
-        <v>0.43968000000000046</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>VO2max!M7</f>
-        <v>70</v>
-      </c>
-      <c r="B4">
-        <f>VO2max!T7*9</f>
-        <v>1.3446719999999994</v>
-      </c>
-      <c r="C4">
-        <f>VO2max!U7*4</f>
-        <v>0.57628800000000047</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A2" s="9">
         <f>VO2max!M8</f>
         <v>80</v>
       </c>
-      <c r="B5">
+      <c r="B2" s="10">
         <f>VO2max!T8*9</f>
         <v>1.4088959999999997</v>
       </c>
-      <c r="C5">
+      <c r="C2" s="10">
         <f>VO2max!U8*4</f>
         <v>0.35222400000000031</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
         <f>VO2max!M9</f>
         <v>84</v>
       </c>
-      <c r="B6">
+      <c r="B3" s="10">
         <f>VO2max!T9*9</f>
         <v>1.6511039999999997</v>
       </c>
-      <c r="C6">
+      <c r="C3" s="10">
         <f>VO2max!U9*4</f>
         <v>0.25401600000000041</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <f>VO2max!M10</f>
         <v>76</v>
       </c>
-      <c r="B7">
+      <c r="B4" s="10">
         <f>VO2max!T10*9</f>
         <v>1.7075999999999996</v>
       </c>
-      <c r="C7">
+      <c r="C4" s="10">
         <f>VO2max!U10*4</f>
         <v>0.34152000000000032</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <f>VO2max!M11</f>
         <v>84</v>
       </c>
-      <c r="B8">
+      <c r="B5" s="10">
         <f>VO2max!T11*9</f>
         <v>2.9329439999999996</v>
       </c>
-      <c r="C8">
+      <c r="C5" s="10">
         <f>VO2max!U11*4</f>
         <v>0.10113599999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <f>VO2max!M12</f>
         <v>92</v>
       </c>
-      <c r="B9">
+      <c r="B6" s="10">
         <f>VO2max!T12*9</f>
         <v>3.5287199999999999</v>
       </c>
-      <c r="C9">
+      <c r="C6" s="10">
         <f>VO2max!U12*4</f>
         <v>0.12167999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <f>VO2max!M13</f>
         <v>84</v>
       </c>
-      <c r="B10">
+      <c r="B7" s="10">
         <f>VO2max!T13*9</f>
         <v>2.809056</v>
       </c>
-      <c r="C10">
+      <c r="C7" s="10">
         <f>VO2max!U13*4</f>
         <v>9.6863999999999978E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
         <f>VO2max!M14</f>
         <v>82</v>
       </c>
-      <c r="B11">
+      <c r="B8" s="10">
         <f>VO2max!T14*9</f>
         <v>3.4027199999999991</v>
       </c>
-      <c r="C11">
+      <c r="C8" s="10">
         <f>VO2max!U14*4</f>
         <v>-0.40031999999999923</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
         <f>VO2max!M15</f>
         <v>88</v>
       </c>
-      <c r="B12">
+      <c r="B9" s="10">
         <f>VO2max!T15*9</f>
         <v>4.8094079999999995</v>
       </c>
-      <c r="C12">
+      <c r="C9" s="10">
         <f>VO2max!U15*4</f>
         <v>-0.90988799999999925</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
         <f>VO2max!M16</f>
         <v>88</v>
       </c>
-      <c r="B13">
+      <c r="B10" s="10">
         <f>VO2max!T16*9</f>
         <v>4.878671999999999</v>
       </c>
-      <c r="C13">
+      <c r="C10" s="10">
         <f>VO2max!U16*4</f>
         <v>-0.92299199999999926</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <f>VO2max!M17</f>
         <v>90</v>
       </c>
-      <c r="B14">
+      <c r="B11" s="10">
         <f>VO2max!T17*9</f>
         <v>5.8661279999999998</v>
       </c>
-      <c r="C14">
+      <c r="C11" s="10">
         <f>VO2max!U17*4</f>
         <v>-1.1098079999999992</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
         <f>VO2max!M18</f>
         <v>94</v>
       </c>
-      <c r="B15">
+      <c r="B12" s="10">
         <f>VO2max!T18*9</f>
         <v>5.9334719999999992</v>
       </c>
-      <c r="C15">
+      <c r="C12" s="10">
         <f>VO2max!U18*4</f>
         <v>-1.2491519999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <f>VO2max!M19</f>
         <v>96</v>
       </c>
-      <c r="B16">
+      <c r="B13" s="10">
         <f>VO2max!T19*9</f>
         <v>7.9756799999999988</v>
       </c>
-      <c r="C16">
+      <c r="C13" s="10">
         <f>VO2max!U19*4</f>
         <v>-1.9939199999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
         <f>VO2max!M20</f>
         <v>99</v>
       </c>
-      <c r="B17">
+      <c r="B14" s="10">
         <f>VO2max!T20*9</f>
         <v>9.7514400000000006</v>
       </c>
-      <c r="C17">
+      <c r="C14" s="10">
         <f>VO2max!U20*4</f>
         <v>-2.6162400000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
         <f>VO2max!M21</f>
         <v>102</v>
       </c>
-      <c r="B18">
+      <c r="B15" s="10">
         <f>VO2max!T21*9</f>
         <v>9.1929599999999994</v>
       </c>
-      <c r="C18">
+      <c r="C15" s="10">
         <f>VO2max!U21*4</f>
         <v>-2.2982399999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
         <f>VO2max!M22</f>
         <v>103</v>
       </c>
-      <c r="B19">
+      <c r="B16" s="10">
         <f>VO2max!T22*9</f>
         <v>11.114880000000003</v>
       </c>
-      <c r="C19">
+      <c r="C16" s="10">
         <f>VO2max!U22*4</f>
         <v>-2.7787199999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
         <f>VO2max!M23</f>
         <v>106</v>
       </c>
-      <c r="B20">
+      <c r="B17" s="10">
         <f>VO2max!T23*9</f>
         <v>10.528128000000002</v>
       </c>
-      <c r="C20">
+      <c r="C17" s="10">
         <f>VO2max!U23*4</f>
         <v>-2.2164479999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
         <f>VO2max!M24</f>
         <v>114</v>
       </c>
-      <c r="B21">
+      <c r="B18" s="10">
         <f>VO2max!T24*9</f>
         <v>8.8490879999999983</v>
       </c>
-      <c r="C21">
+      <c r="C18" s="10">
         <f>VO2max!U24*4</f>
         <v>-1.4748479999999982</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
         <f>VO2max!M25</f>
         <v>106</v>
       </c>
-      <c r="B22">
+      <c r="B19" s="10">
         <f>VO2max!T25*9</f>
         <v>9.9859199999999984</v>
       </c>
-      <c r="C22">
+      <c r="C19" s="10">
         <f>VO2max!U25*4</f>
         <v>-1.4265599999999987</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
         <f>VO2max!M26</f>
         <v>109</v>
       </c>
-      <c r="B23">
+      <c r="B20" s="10">
         <f>VO2max!T26*9</f>
         <v>11.872559999999998</v>
       </c>
-      <c r="C23">
+      <c r="C20" s="10">
         <f>VO2max!U26*4</f>
         <v>-1.6960799999999985</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
         <f>VO2max!M27</f>
         <v>117</v>
       </c>
-      <c r="B24">
+      <c r="B21" s="10">
         <f>VO2max!T27*9</f>
         <v>10.959839999999998</v>
       </c>
-      <c r="C24">
+      <c r="C21" s="10">
         <f>VO2max!U27*4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
         <f>VO2max!M28</f>
         <v>124</v>
       </c>
-      <c r="B25">
+      <c r="B22" s="10">
         <f>VO2max!T28*9</f>
         <v>10.771055999999998</v>
       </c>
-      <c r="C25">
+      <c r="C22" s="10">
         <f>VO2max!U28*4</f>
         <v>1.196784000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
         <f>VO2max!M29</f>
         <v>126</v>
       </c>
-      <c r="B26">
+      <c r="B23" s="10">
         <f>VO2max!T29*9</f>
         <v>9.178799999999999</v>
       </c>
-      <c r="C26">
+      <c r="C23" s="10">
         <f>VO2max!U29*4</f>
         <v>1.8357600000000023</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
         <f>VO2max!M30</f>
         <v>129</v>
       </c>
-      <c r="B27">
+      <c r="B24" s="10">
         <f>VO2max!T30*9</f>
         <v>9.6455999999999964</v>
       </c>
-      <c r="C27">
+      <c r="C24" s="10">
         <f>VO2max!U30*4</f>
         <v>1.9291200000000019</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
         <f>VO2max!M31</f>
         <v>135</v>
       </c>
-      <c r="B28">
+      <c r="B25" s="10">
         <f>VO2max!T31*9</f>
         <v>10.481375999999996</v>
       </c>
-      <c r="C28">
+      <c r="C25" s="10">
         <f>VO2max!U31*4</f>
         <v>3.1899840000000039</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
         <f>VO2max!M32</f>
         <v>138</v>
       </c>
-      <c r="B29">
+      <c r="B26" s="10">
         <f>VO2max!T32*9</f>
         <v>7.8321599999999991</v>
       </c>
-      <c r="C29">
+      <c r="C26" s="10">
         <f>VO2max!U32*4</f>
         <v>5.2214400000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
         <f>VO2max!M33</f>
         <v>148</v>
       </c>
-      <c r="B30">
+      <c r="B27" s="10">
         <f>VO2max!T33*9</f>
         <v>8.0180159999999994</v>
       </c>
-      <c r="C30">
+      <c r="C27" s="10">
         <f>VO2max!U33*4</f>
         <v>6.131424</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
         <f>VO2max!M34</f>
         <v>139</v>
       </c>
-      <c r="B31">
+      <c r="B28" s="10">
         <f>VO2max!T34*9</f>
         <v>6.9573119999999991</v>
       </c>
-      <c r="C31">
+      <c r="C28" s="10">
         <f>VO2max!U34*4</f>
         <v>6.0876480000000024</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
         <f>VO2max!M35</f>
         <v>143</v>
       </c>
-      <c r="B32">
+      <c r="B29" s="10">
         <f>VO2max!T35*9</f>
         <v>8.2974719999999973</v>
       </c>
-      <c r="C32">
+      <c r="C29" s="10">
         <f>VO2max!U35*4</f>
         <v>7.2602880000000019</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
         <f>VO2max!M36</f>
         <v>149</v>
       </c>
-      <c r="B33">
+      <c r="B30" s="10">
         <f>VO2max!T36*9</f>
         <v>5.2545599999999952</v>
       </c>
-      <c r="C33">
+      <c r="C30" s="10">
         <f>VO2max!U36*4</f>
         <v>10.509120000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <f>VO2max!M37</f>
         <v>155</v>
       </c>
-      <c r="B34">
+      <c r="B31" s="10">
         <f>VO2max!T37*9</f>
         <v>3.7339679999999928</v>
       </c>
-      <c r="C34">
+      <c r="C31" s="10">
         <f>VO2max!U37*4</f>
         <v>12.268752000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
         <f>VO2max!M38</f>
         <v>158</v>
       </c>
-      <c r="B35">
+      <c r="B32" s="10">
         <f>VO2max!T38*9</f>
         <v>2.3767679999999993</v>
       </c>
-      <c r="C35">
+      <c r="C32" s="10">
         <f>VO2max!U38*4</f>
         <v>15.448992000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
         <f>VO2max!M39</f>
         <v>161</v>
       </c>
-      <c r="B36">
+      <c r="B33" s="10">
         <f>VO2max!T39*9</f>
         <v>0.58747199999999777</v>
       </c>
-      <c r="C36">
+      <c r="C33" s="10">
         <f>VO2max!U39*4</f>
         <v>17.036688000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
         <f>VO2max!M40</f>
         <v>165</v>
       </c>
-      <c r="B37">
+      <c r="B34" s="10">
         <f>VO2max!T40*9</f>
         <v>-2.4595200000000075</v>
       </c>
-      <c r="C37">
+      <c r="C34" s="10">
         <f>VO2max!U40*4</f>
         <v>20.905920000000009</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
         <f>VO2max!M41</f>
         <v>167</v>
       </c>
-      <c r="B38">
+      <c r="B35" s="10">
         <f>VO2max!T41*9</f>
         <v>-2.5288320000000075</v>
       </c>
-      <c r="C38">
+      <c r="C35" s="10">
         <f>VO2max!U41*4</f>
         <v>21.495072000000008</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
         <f>VO2max!M42</f>
         <v>169</v>
       </c>
-      <c r="B39">
+      <c r="B36" s="10">
         <f>VO2max!T42*9</f>
         <v>-5.0465280000000075</v>
       </c>
-      <c r="C39">
+      <c r="C36" s="10">
         <f>VO2max!U42*4</f>
         <v>23.971008000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
         <f>VO2max!M43</f>
         <v>173</v>
       </c>
-      <c r="B40">
+      <c r="B37" s="10">
         <f>VO2max!T43*9</f>
         <v>-4.6958400000000076</v>
       </c>
-      <c r="C40">
+      <c r="C37" s="10">
         <f>VO2max!U43*4</f>
         <v>20.348640000000007</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
         <f>VO2max!M44</f>
         <v>170</v>
       </c>
-      <c r="B41">
+      <c r="B38" s="10">
         <f>VO2max!T44*9</f>
         <v>-4.7266560000000073</v>
       </c>
-      <c r="C41">
+      <c r="C38" s="10">
         <f>VO2max!U44*4</f>
         <v>22.451616000000005</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <f>VO2max!M45</f>
-        <v>161</v>
-      </c>
-      <c r="B42">
-        <f>VO2max!T45*9</f>
-        <v>-3.2699040000000039</v>
-      </c>
-      <c r="C42">
-        <f>VO2max!U45*4</f>
-        <v>12.187824000000003</v>
       </c>
     </row>
   </sheetData>
@@ -10335,11 +10435,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10362,518 +10460,504 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <f>VO2max!W5</f>
-        <v>0.12280701754385964</v>
+        <f>VO2max!W6</f>
+        <v>9.0643274853801165E-2</v>
       </c>
       <c r="B2">
-        <f>VO2max!T5*9</f>
-        <v>1.9452959999999999</v>
+        <f>VO2max!T6*9</f>
+        <v>1.2091199999999995</v>
       </c>
       <c r="C2">
-        <f>VO2max!U5*4</f>
-        <v>0.21614400000000022</v>
+        <f>VO2max!U6*4</f>
+        <v>0.43968000000000046</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <f>VO2max!W6</f>
-        <v>9.0643274853801165E-2</v>
+        <f>VO2max!W7</f>
+        <v>0.10818713450292397</v>
       </c>
       <c r="B3">
-        <f>VO2max!T6*9</f>
-        <v>1.2091199999999995</v>
+        <f>VO2max!T7*9</f>
+        <v>1.3446719999999994</v>
       </c>
       <c r="C3">
-        <f>VO2max!U6*4</f>
-        <v>0.43968000000000046</v>
+        <f>VO2max!U7*4</f>
+        <v>0.57628800000000047</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <f>VO2max!W7</f>
-        <v>0.10818713450292397</v>
+        <f>VO2max!W8</f>
+        <v>9.6491228070175419E-2</v>
       </c>
       <c r="B4">
-        <f>VO2max!T7*9</f>
-        <v>1.3446719999999994</v>
+        <f>VO2max!T8*9</f>
+        <v>1.4088959999999997</v>
       </c>
       <c r="C4">
-        <f>VO2max!U7*4</f>
-        <v>0.57628800000000047</v>
+        <f>VO2max!U8*4</f>
+        <v>0.35222400000000031</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>VO2max!W8</f>
-        <v>9.6491228070175419E-2</v>
+        <f>VO2max!W9</f>
+        <v>0.10526315789473684</v>
       </c>
       <c r="B5">
-        <f>VO2max!T8*9</f>
-        <v>1.4088959999999997</v>
+        <f>VO2max!T9*9</f>
+        <v>1.6511039999999997</v>
       </c>
       <c r="C5">
-        <f>VO2max!U8*4</f>
-        <v>0.35222400000000031</v>
+        <f>VO2max!U9*4</f>
+        <v>0.25401600000000041</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <f>VO2max!W9</f>
-        <v>0.10526315789473684</v>
+        <f>VO2max!W10</f>
+        <v>0.11695906432748537</v>
       </c>
       <c r="B6">
-        <f>VO2max!T9*9</f>
-        <v>1.6511039999999997</v>
+        <f>VO2max!T10*9</f>
+        <v>1.7075999999999996</v>
       </c>
       <c r="C6">
-        <f>VO2max!U9*4</f>
-        <v>0.25401600000000041</v>
+        <f>VO2max!U10*4</f>
+        <v>0.34152000000000032</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <f>VO2max!W10</f>
-        <v>0.11695906432748537</v>
+        <f>VO2max!W11</f>
+        <v>0.17251461988304093</v>
       </c>
       <c r="B7">
-        <f>VO2max!T10*9</f>
-        <v>1.7075999999999996</v>
+        <f>VO2max!T11*9</f>
+        <v>2.9329439999999996</v>
       </c>
       <c r="C7">
-        <f>VO2max!U10*4</f>
-        <v>0.34152000000000032</v>
+        <f>VO2max!U11*4</f>
+        <v>0.10113599999999996</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <f>VO2max!W11</f>
-        <v>0.17251461988304093</v>
+        <f>VO2max!W12</f>
+        <v>0.20760233918128651</v>
       </c>
       <c r="B8">
-        <f>VO2max!T11*9</f>
-        <v>2.9329439999999996</v>
+        <f>VO2max!T12*9</f>
+        <v>3.5287199999999999</v>
       </c>
       <c r="C8">
-        <f>VO2max!U11*4</f>
-        <v>0.10113599999999996</v>
+        <f>VO2max!U12*4</f>
+        <v>0.12167999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <f>VO2max!W12</f>
-        <v>0.20760233918128651</v>
+        <f>VO2max!W13</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="B9">
-        <f>VO2max!T12*9</f>
-        <v>3.5287199999999999</v>
+        <f>VO2max!T13*9</f>
+        <v>2.809056</v>
       </c>
       <c r="C9">
-        <f>VO2max!U12*4</f>
-        <v>0.12167999999999997</v>
+        <f>VO2max!U13*4</f>
+        <v>9.6863999999999978E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <f>VO2max!W13</f>
-        <v>0.16666666666666666</v>
+        <f>VO2max!W14</f>
+        <v>0.17251461988304093</v>
       </c>
       <c r="B10">
-        <f>VO2max!T13*9</f>
-        <v>2.809056</v>
+        <f>VO2max!T14*9</f>
+        <v>3.4027199999999991</v>
       </c>
       <c r="C10">
-        <f>VO2max!U13*4</f>
-        <v>9.6863999999999978E-2</v>
+        <f>VO2max!U14*4</f>
+        <v>-0.40031999999999923</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <f>VO2max!W14</f>
-        <v>0.17251461988304093</v>
+        <f>VO2max!W15</f>
+        <v>0.22807017543859648</v>
       </c>
       <c r="B11">
-        <f>VO2max!T14*9</f>
-        <v>3.4027199999999991</v>
+        <f>VO2max!T15*9</f>
+        <v>4.8094079999999995</v>
       </c>
       <c r="C11">
-        <f>VO2max!U14*4</f>
-        <v>-0.40031999999999923</v>
+        <f>VO2max!U15*4</f>
+        <v>-0.90988799999999925</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <f>VO2max!W15</f>
+        <f>VO2max!W16</f>
         <v>0.22807017543859648</v>
       </c>
       <c r="B12">
-        <f>VO2max!T15*9</f>
-        <v>4.8094079999999995</v>
+        <f>VO2max!T16*9</f>
+        <v>4.878671999999999</v>
       </c>
       <c r="C12">
-        <f>VO2max!U15*4</f>
-        <v>-0.90988799999999925</v>
+        <f>VO2max!U16*4</f>
+        <v>-0.92299199999999926</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <f>VO2max!W16</f>
-        <v>0.22807017543859648</v>
+        <f>VO2max!W17</f>
+        <v>0.27777777777777773</v>
       </c>
       <c r="B13">
-        <f>VO2max!T16*9</f>
-        <v>4.878671999999999</v>
+        <f>VO2max!T17*9</f>
+        <v>5.8661279999999998</v>
       </c>
       <c r="C13">
-        <f>VO2max!U16*4</f>
-        <v>-0.92299199999999926</v>
+        <f>VO2max!U17*4</f>
+        <v>-1.1098079999999992</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <f>VO2max!W17</f>
-        <v>0.27777777777777773</v>
+        <f>VO2max!W18</f>
+        <v>0.27192982456140352</v>
       </c>
       <c r="B14">
-        <f>VO2max!T17*9</f>
-        <v>5.8661279999999998</v>
+        <f>VO2max!T18*9</f>
+        <v>5.9334719999999992</v>
       </c>
       <c r="C14">
-        <f>VO2max!U17*4</f>
-        <v>-1.1098079999999992</v>
+        <f>VO2max!U18*4</f>
+        <v>-1.2491519999999996</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <f>VO2max!W18</f>
-        <v>0.27192982456140352</v>
+        <f>VO2max!W19</f>
+        <v>0.34795321637426901</v>
       </c>
       <c r="B15">
-        <f>VO2max!T18*9</f>
-        <v>5.9334719999999992</v>
+        <f>VO2max!T19*9</f>
+        <v>7.9756799999999988</v>
       </c>
       <c r="C15">
-        <f>VO2max!U18*4</f>
-        <v>-1.2491519999999996</v>
+        <f>VO2max!U19*4</f>
+        <v>-1.9939199999999995</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <f>VO2max!W19</f>
-        <v>0.34795321637426901</v>
+        <f>VO2max!W20</f>
+        <v>0.41812865497076024</v>
       </c>
       <c r="B16">
-        <f>VO2max!T19*9</f>
-        <v>7.9756799999999988</v>
+        <f>VO2max!T20*9</f>
+        <v>9.7514400000000006</v>
       </c>
       <c r="C16">
-        <f>VO2max!U19*4</f>
-        <v>-1.9939199999999995</v>
+        <f>VO2max!U20*4</f>
+        <v>-2.6162400000000003</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <f>VO2max!W20</f>
-        <v>0.41812865497076024</v>
+        <f>VO2max!W21</f>
+        <v>0.40350877192982454</v>
       </c>
       <c r="B17">
-        <f>VO2max!T20*9</f>
-        <v>9.7514400000000006</v>
+        <f>VO2max!T21*9</f>
+        <v>9.1929599999999994</v>
       </c>
       <c r="C17">
-        <f>VO2max!U20*4</f>
-        <v>-2.6162400000000003</v>
+        <f>VO2max!U21*4</f>
+        <v>-2.2982399999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
-        <f>VO2max!W21</f>
-        <v>0.40350877192982454</v>
+        <f>VO2max!W22</f>
+        <v>0.48538011695906436</v>
       </c>
       <c r="B18">
-        <f>VO2max!T21*9</f>
-        <v>9.1929599999999994</v>
+        <f>VO2max!T22*9</f>
+        <v>11.114880000000003</v>
       </c>
       <c r="C18">
-        <f>VO2max!U21*4</f>
-        <v>-2.2982399999999998</v>
+        <f>VO2max!U22*4</f>
+        <v>-2.7787199999999999</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <f>VO2max!W22</f>
-        <v>0.48538011695906436</v>
+        <f>VO2max!W23</f>
+        <v>0.48245614035087714</v>
       </c>
       <c r="B19">
-        <f>VO2max!T22*9</f>
-        <v>11.114880000000003</v>
+        <f>VO2max!T23*9</f>
+        <v>10.528128000000002</v>
       </c>
       <c r="C19">
-        <f>VO2max!U22*4</f>
-        <v>-2.7787199999999999</v>
+        <f>VO2max!U23*4</f>
+        <v>-2.2164479999999998</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <f>VO2max!W23</f>
-        <v>0.48245614035087714</v>
+        <f>VO2max!W24</f>
+        <v>0.42690058479532161</v>
       </c>
       <c r="B20">
-        <f>VO2max!T23*9</f>
-        <v>10.528128000000002</v>
+        <f>VO2max!T24*9</f>
+        <v>8.8490879999999983</v>
       </c>
       <c r="C20">
-        <f>VO2max!U23*4</f>
-        <v>-2.2164479999999998</v>
+        <f>VO2max!U24*4</f>
+        <v>-1.4748479999999982</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <f>VO2max!W24</f>
-        <v>0.42690058479532161</v>
+        <f>VO2max!W25</f>
+        <v>0.49122807017543857</v>
       </c>
       <c r="B21">
-        <f>VO2max!T24*9</f>
-        <v>8.8490879999999983</v>
+        <f>VO2max!T25*9</f>
+        <v>9.9859199999999984</v>
       </c>
       <c r="C21">
-        <f>VO2max!U24*4</f>
-        <v>-1.4748479999999982</v>
+        <f>VO2max!U25*4</f>
+        <v>-1.4265599999999987</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <f>VO2max!W25</f>
-        <v>0.49122807017543857</v>
+        <f>VO2max!W26</f>
+        <v>0.58771929824561397</v>
       </c>
       <c r="B22">
-        <f>VO2max!T25*9</f>
-        <v>9.9859199999999984</v>
+        <f>VO2max!T26*9</f>
+        <v>11.872559999999998</v>
       </c>
       <c r="C22">
-        <f>VO2max!U25*4</f>
-        <v>-1.4265599999999987</v>
+        <f>VO2max!U26*4</f>
+        <v>-1.6960799999999985</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <f>VO2max!W26</f>
-        <v>0.58771929824561397</v>
+        <f>VO2max!W27</f>
+        <v>0.62573099415204669</v>
       </c>
       <c r="B23">
-        <f>VO2max!T26*9</f>
-        <v>11.872559999999998</v>
+        <f>VO2max!T27*9</f>
+        <v>10.959839999999998</v>
       </c>
       <c r="C23">
-        <f>VO2max!U26*4</f>
-        <v>-1.6960799999999985</v>
+        <f>VO2max!U27*4</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <f>VO2max!W27</f>
-        <v>0.62573099415204669</v>
+        <f>VO2max!W28</f>
+        <v>0.67836257309941517</v>
       </c>
       <c r="B24">
-        <f>VO2max!T27*9</f>
-        <v>10.959839999999998</v>
+        <f>VO2max!T28*9</f>
+        <v>10.771055999999998</v>
       </c>
       <c r="C24">
-        <f>VO2max!U27*4</f>
-        <v>0</v>
+        <f>VO2max!U28*4</f>
+        <v>1.196784000000001</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <f>VO2max!W28</f>
-        <v>0.67836257309941517</v>
+        <f>VO2max!W29</f>
+        <v>0.62280701754385959</v>
       </c>
       <c r="B25">
-        <f>VO2max!T28*9</f>
-        <v>10.771055999999998</v>
+        <f>VO2max!T29*9</f>
+        <v>9.178799999999999</v>
       </c>
       <c r="C25">
-        <f>VO2max!U28*4</f>
-        <v>1.196784000000001</v>
+        <f>VO2max!U29*4</f>
+        <v>1.8357600000000023</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <f>VO2max!W29</f>
-        <v>0.62280701754385959</v>
+        <f>VO2max!W30</f>
+        <v>0.64912280701754377</v>
       </c>
       <c r="B26">
-        <f>VO2max!T29*9</f>
-        <v>9.178799999999999</v>
+        <f>VO2max!T30*9</f>
+        <v>9.6455999999999964</v>
       </c>
       <c r="C26">
-        <f>VO2max!U29*4</f>
-        <v>1.8357600000000023</v>
+        <f>VO2max!U30*4</f>
+        <v>1.9291200000000019</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <f>VO2max!W30</f>
-        <v>0.64912280701754377</v>
+        <f>VO2max!W31</f>
+        <v>0.76608187134502914</v>
       </c>
       <c r="B27">
-        <f>VO2max!T30*9</f>
-        <v>9.6455999999999964</v>
+        <f>VO2max!T31*9</f>
+        <v>10.481375999999996</v>
       </c>
       <c r="C27">
-        <f>VO2max!U30*4</f>
-        <v>1.9291200000000019</v>
+        <f>VO2max!U31*4</f>
+        <v>3.1899840000000039</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <f>VO2max!W31</f>
-        <v>0.76608187134502914</v>
+        <f>VO2max!W32</f>
+        <v>0.72514619883040932</v>
       </c>
       <c r="B28">
-        <f>VO2max!T31*9</f>
-        <v>10.481375999999996</v>
+        <f>VO2max!T32*9</f>
+        <v>7.8321599999999991</v>
       </c>
       <c r="C28">
-        <f>VO2max!U31*4</f>
-        <v>3.1899840000000039</v>
+        <f>VO2max!U32*4</f>
+        <v>5.2214400000000003</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <f>VO2max!W32</f>
-        <v>0.72514619883040932</v>
+        <f>VO2max!W33</f>
+        <v>0.78070175438596479</v>
       </c>
       <c r="B29">
-        <f>VO2max!T32*9</f>
-        <v>7.8321599999999991</v>
+        <f>VO2max!T33*9</f>
+        <v>8.0180159999999994</v>
       </c>
       <c r="C29">
-        <f>VO2max!U32*4</f>
-        <v>5.2214400000000003</v>
+        <f>VO2max!U33*4</f>
+        <v>6.131424</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <f>VO2max!W33</f>
-        <v>0.78070175438596479</v>
+        <f>VO2max!W34</f>
+        <v>0.7192982456140351</v>
       </c>
       <c r="B30">
-        <f>VO2max!T33*9</f>
-        <v>8.0180159999999994</v>
+        <f>VO2max!T34*9</f>
+        <v>6.9573119999999991</v>
       </c>
       <c r="C30">
-        <f>VO2max!U33*4</f>
-        <v>6.131424</v>
+        <f>VO2max!U34*4</f>
+        <v>6.0876480000000024</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <f>VO2max!W34</f>
-        <v>0.7192982456140351</v>
+        <f>VO2max!W35</f>
+        <v>0.85964912280701744</v>
       </c>
       <c r="B31">
-        <f>VO2max!T34*9</f>
-        <v>6.9573119999999991</v>
+        <f>VO2max!T35*9</f>
+        <v>8.2974719999999973</v>
       </c>
       <c r="C31">
-        <f>VO2max!U34*4</f>
-        <v>6.0876480000000024</v>
+        <f>VO2max!U35*4</f>
+        <v>7.2602880000000019</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <f>VO2max!W35</f>
+        <f>VO2max!W36</f>
         <v>0.85964912280701744</v>
       </c>
       <c r="B32">
-        <f>VO2max!T35*9</f>
-        <v>8.2974719999999973</v>
+        <f>VO2max!T36*9</f>
+        <v>5.2545599999999952</v>
       </c>
       <c r="C32">
-        <f>VO2max!U35*4</f>
-        <v>7.2602880000000019</v>
+        <f>VO2max!U36*4</f>
+        <v>10.509120000000005</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <f>VO2max!W36</f>
-        <v>0.85964912280701744</v>
+        <f>VO2max!W37</f>
+        <v>0.86257309941520466</v>
       </c>
       <c r="B33">
-        <f>VO2max!T36*9</f>
-        <v>5.2545599999999952</v>
+        <f>VO2max!T37*9</f>
+        <v>3.7339679999999928</v>
       </c>
       <c r="C33">
-        <f>VO2max!U36*4</f>
-        <v>10.509120000000005</v>
+        <f>VO2max!U37*4</f>
+        <v>12.268752000000003</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <f>VO2max!W37</f>
-        <v>0.86257309941520466</v>
+        <f>VO2max!W38</f>
+        <v>0.95614035087719296</v>
       </c>
       <c r="B34">
-        <f>VO2max!T37*9</f>
-        <v>3.7339679999999928</v>
+        <f>VO2max!T38*9</f>
+        <v>2.3767679999999993</v>
       </c>
       <c r="C34">
-        <f>VO2max!U37*4</f>
-        <v>12.268752000000003</v>
+        <f>VO2max!U38*4</f>
+        <v>15.448992000000002</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
-        <f>VO2max!W38</f>
-        <v>0.95614035087719296</v>
+        <f>VO2max!W39</f>
+        <v>0.9385964912280701</v>
       </c>
       <c r="B35">
-        <f>VO2max!T38*9</f>
-        <v>2.3767679999999993</v>
+        <f>VO2max!T39*9</f>
+        <v>0.58747199999999777</v>
       </c>
       <c r="C35">
-        <f>VO2max!U38*4</f>
-        <v>15.448992000000002</v>
+        <f>VO2max!U39*4</f>
+        <v>17.036688000000002</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <f>VO2max!W39</f>
-        <v>0.9385964912280701</v>
+        <f>VO2max!W40</f>
+        <v>0.97076023391812871</v>
       </c>
       <c r="B36">
-        <f>VO2max!T39*9</f>
-        <v>0.58747199999999777</v>
+        <f>VO2max!T40*9</f>
+        <v>-2.4595200000000075</v>
       </c>
       <c r="C36">
-        <f>VO2max!U39*4</f>
-        <v>17.036688000000002</v>
+        <f>VO2max!U40*4</f>
+        <v>20.905920000000009</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <f>VO2max!W40</f>
-        <v>0.97076023391812871</v>
-      </c>
-      <c r="B37">
-        <f>VO2max!T40*9</f>
-        <v>-2.4595200000000075</v>
-      </c>
-      <c r="C37">
-        <f>VO2max!U40*4</f>
-        <v>20.905920000000009</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
         <f>VO2max!W41</f>
         <v>1</v>
       </c>
-      <c r="B38">
+      <c r="B37">
         <f>VO2max!T41*9</f>
         <v>-2.5288320000000075</v>
       </c>
-      <c r="C38">
+      <c r="C37">
         <f>VO2max!U41*4</f>
         <v>21.495072000000008</v>
       </c>

</xml_diff>